<commit_message>
Week 6 - Day 1 - Assignment 1
</commit_message>
<xml_diff>
--- a/MavenProject/data/Lead.xlsx
+++ b/MavenProject/data/Lead.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
-    <sheet name="contact" sheetId="2" r:id="rId2"/>
+    <sheet name="companies" sheetId="2" r:id="rId2"/>
     <sheet name="leads" sheetId="3" r:id="rId3"/>
+    <sheet name="contact" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>CompanyName</t>
   </si>
@@ -63,12 +64,21 @@
     <t>Phone</t>
   </si>
   <si>
+    <t>Company</t>
+  </si>
+  <si>
     <t>97</t>
   </si>
   <si>
+    <t>TCS</t>
+  </si>
+  <si>
     <t>98</t>
   </si>
   <si>
+    <t>Wipro</t>
+  </si>
+  <si>
     <t>87</t>
   </si>
   <si>
@@ -84,7 +94,7 @@
     <t>babu</t>
   </si>
   <si>
-    <t>Azim</t>
+    <t>pavi</t>
   </si>
 </sst>
 </file>
@@ -1106,35 +1116,47 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="10.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1171,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
@@ -1159,26 +1181,63 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>